<commit_message>
Actualización cuaderno de estudio tema  4 grado 8
Se actualiza el cuaderno de estudio de acuerdo a la escaleta final.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion04/SolicitudGrafica-MA_08_04_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion04/SolicitudGrafica-MA_08_04_CO.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="156">
   <si>
     <t>Fecha:</t>
   </si>
@@ -526,34 +526,16 @@
     <t>IMG03</t>
   </si>
   <si>
-    <t>IMG04</t>
-  </si>
-  <si>
-    <t>IMG05</t>
-  </si>
-  <si>
-    <t>IMG06</t>
-  </si>
-  <si>
     <t>Factorización</t>
   </si>
   <si>
     <t>MA_08_04_CO</t>
   </si>
   <si>
-    <t>Esta imagen no se va a ubicar en el interior de un recuadro y no tendra pie de imagen, por ello no olvidar agregar el texto al lado de la imagen.</t>
-  </si>
-  <si>
-    <t>Esta es una imagen de acompañamiento, recortarla y dejar solo la parte que se muestra en observaciones, quitar el fondo gris de la imagen.</t>
-  </si>
-  <si>
-    <t>Imagen de acompañamiento, quitar el fondo.</t>
-  </si>
-  <si>
-    <t>imagen de acompañamiento, no se ubica en el interior del recuadro de imagen y no tiene pie de imagen.</t>
-  </si>
-  <si>
-    <t>Imagen de acompañamiento.</t>
+    <t>Agregar cotas</t>
+  </si>
+  <si>
+    <t>No olvidar agregar el texto al lado de la imagen.</t>
   </si>
 </sst>
 </file>
@@ -1691,13 +1673,13 @@
           <xdr:col>10</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>258535</xdr:rowOff>
+          <xdr:rowOff>257175</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>4657725</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>1820635</xdr:rowOff>
+          <xdr:rowOff>1819275</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1738,19 +1720,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1927771</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>4029075</xdr:colOff>
+      <xdr:colOff>1364796</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>2068287</xdr:rowOff>
+      <xdr:rowOff>1367518</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Imagen 17"/>
+        <xdr:cNvPr id="8" name="Imagen 7"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1770,8 +1752,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="22052735" y="4327072"/>
-          <a:ext cx="2101304" cy="2068286"/>
+          <a:off x="20124964" y="4327071"/>
+          <a:ext cx="1364796" cy="1367518"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1793,19 +1775,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1711086</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>163286</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3524249</xdr:colOff>
+      <xdr:colOff>2042999</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>2058761</xdr:rowOff>
+      <xdr:rowOff>1796142</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Imagen 20" descr="Balance icon"/>
+        <xdr:cNvPr id="9" name="Imagen 8"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1825,165 +1807,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="21836050" y="6585857"/>
-          <a:ext cx="1813163" cy="1895475"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1442356</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>4286249</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>1782536</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Imagen 21" descr="Montessori Materials. Binomial Cube. "/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21567320" y="8518071"/>
-          <a:ext cx="2843893" cy="1782536"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1129393</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>217714</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>3172392</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>2013856</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Imagen 23"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21254357" y="12627428"/>
+          <a:off x="20124964" y="6422571"/>
           <a:ext cx="2042999" cy="1796142"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1605643</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>367392</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>2970439</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>1734910</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Imagen 24"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21730607" y="10899321"/>
-          <a:ext cx="1364796" cy="1367518"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2722,7 +2547,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2793,7 +2618,7 @@
         <v>54</v>
       </c>
       <c r="C4" s="87" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D4" s="88"/>
       <c r="E4" s="5"/>
@@ -2849,7 +2674,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D7" s="36" t="s">
         <v>39</v>
@@ -2951,7 +2776,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K10"/>
     </row>
@@ -2963,7 +2788,7 @@
         <v>241287070</v>
       </c>
       <c r="C11" s="26" t="str">
-        <f t="shared" ref="C11:C18" si="0">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <f t="shared" ref="C11:C14" si="0">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D11" s="14" t="s">
@@ -2989,7 +2814,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J11" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="K11" s="19"/>
     </row>
@@ -3026,122 +2851,46 @@
         <f>IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J12" t="s">
-        <v>159</v>
-      </c>
+      <c r="J12"/>
       <c r="K12"/>
     </row>
     <row r="13" spans="1:16" s="12" customFormat="1" ht="158.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="B13" s="28">
-        <v>262509938</v>
-      </c>
-      <c r="C13" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v>Cuaderno de Estudio</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F13" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>MA_08_04_CO_IMG04_small</v>
-      </c>
-      <c r="G13" s="14" t="str">
-        <f>IF(F13&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>526 x 370 px</v>
-      </c>
-      <c r="H13" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>MA_08_04_CO_IMG04_zoom</v>
-      </c>
-      <c r="I13" s="14" t="str">
-        <f>IF(OR(B13&lt;&gt;"",J13&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J13" t="s">
-        <v>160</v>
-      </c>
+      <c r="A13" s="13"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13"/>
       <c r="K13" s="19"/>
     </row>
     <row r="14" spans="1:16" s="12" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="B14" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="C14" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v>Cuaderno de Estudio</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F14" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>MA_08_04_CO_IMG05_small</v>
-      </c>
-      <c r="G14" s="14" t="str">
-        <f>IF(F14&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>526 x 370 px</v>
-      </c>
-      <c r="H14" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>MA_08_04_CO_IMG05_zoom</v>
-      </c>
-      <c r="I14" s="14" t="str">
-        <f>IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J14" t="s">
-        <v>161</v>
-      </c>
+      <c r="A14" s="13"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14"/>
       <c r="K14" s="19"/>
     </row>
     <row r="15" spans="1:16" s="12" customFormat="1" ht="165" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F15" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>MA_08_04_CO_IMG06_small</v>
-      </c>
-      <c r="G15" s="14" t="str">
-        <f>IF(F15&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>526 x 370 px</v>
-      </c>
-      <c r="H15" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>MA_08_04_CO_IMG06_zoom</v>
-      </c>
-      <c r="I15" s="14" t="str">
-        <f>IF(OR(B15&lt;&gt;"",J15&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J15" t="s">
-        <v>161</v>
-      </c>
+      <c r="A15" s="13"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15"/>
       <c r="K15"/>
     </row>
     <row r="16" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>